<commit_message>
Death Knight Plague finish
</commit_message>
<xml_diff>
--- a/data/Hero_resistance.xlsx
+++ b/data/Hero_resistance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Projects\Legends of Champions Tactics_Git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5CC1E6-A301-4820-A31F-0CE028F634EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566C821C-7542-4AAC-AF03-0C9BE15F5601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1065,22 +1065,22 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2015,7 +2015,7 @@
       </c>
       <c r="I3" s="5">
         <f>'Resistance List'!Q7</f>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J3" s="5">
         <f>'Resistance List'!S7</f>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="I5" s="5">
         <f>'Resistance List'!Q13</f>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J5" s="5">
         <f>'Resistance List'!S13</f>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="I6" s="5">
         <f>'Resistance List'!Q16</f>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J6" s="5">
         <f>'Resistance List'!S16</f>
@@ -2279,7 +2279,7 @@
       </c>
       <c r="I7" s="5">
         <f>'Resistance List'!Q19</f>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J7" s="5">
         <f>'Resistance List'!S19</f>
@@ -2345,7 +2345,7 @@
       </c>
       <c r="I8" s="5">
         <f>'Resistance List'!Q22</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J8" s="5">
         <f>'Resistance List'!S22</f>
@@ -29918,7 +29918,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R10" sqref="R10"/>
+      <selection pane="bottomRight" activeCell="Q11" sqref="Q11:R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -30281,10 +30281,10 @@
         <v>25</v>
       </c>
       <c r="Q5" s="8">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="R5" s="8">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="S5" s="8">
         <v>40</v>
@@ -30349,10 +30349,10 @@
         <v>15</v>
       </c>
       <c r="Q6" s="8">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R6" s="8">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="S6" s="8">
         <v>30</v>
@@ -30433,9 +30433,10 @@
       </c>
       <c r="Q7" s="14">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="R7" s="14">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="S7" s="14">
@@ -30730,10 +30731,10 @@
         <v>50</v>
       </c>
       <c r="Q11" s="8">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="R11" s="8">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="S11" s="8">
         <v>40</v>
@@ -30798,10 +30799,10 @@
         <v>40</v>
       </c>
       <c r="Q12" s="8">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R12" s="8">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S12" s="8">
         <v>30</v>
@@ -30882,9 +30883,10 @@
       </c>
       <c r="Q13" s="14">
         <f t="shared" si="5"/>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="R13" s="14">
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="S13" s="14">
@@ -30954,10 +30956,10 @@
         <v>40</v>
       </c>
       <c r="Q14" s="8">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="R14" s="8">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="S14" s="8">
         <v>35</v>
@@ -31022,10 +31024,10 @@
         <v>30</v>
       </c>
       <c r="Q15" s="8">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R15" s="8">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S15" s="8">
         <v>25</v>
@@ -31106,9 +31108,10 @@
       </c>
       <c r="Q16" s="14">
         <f t="shared" si="6"/>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="R16" s="14">
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="S16" s="14">
@@ -31178,10 +31181,10 @@
         <v>45</v>
       </c>
       <c r="Q17" s="8">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="R17" s="8">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="S17" s="8">
         <v>30</v>
@@ -31246,10 +31249,10 @@
         <v>35</v>
       </c>
       <c r="Q18" s="8">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="R18" s="8">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S18" s="8">
         <v>20</v>
@@ -31330,9 +31333,10 @@
       </c>
       <c r="Q19" s="14">
         <f t="shared" si="7"/>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="R19" s="14">
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="S19" s="14">
@@ -31402,10 +31406,10 @@
         <v>35</v>
       </c>
       <c r="Q20" s="8">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="R20" s="8">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="S20" s="8">
         <v>30</v>
@@ -31470,10 +31474,10 @@
         <v>25</v>
       </c>
       <c r="Q21" s="8">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="R21" s="8">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="S21" s="8">
         <v>20</v>
@@ -31554,9 +31558,10 @@
       </c>
       <c r="Q22" s="14">
         <f t="shared" si="8"/>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="R22" s="14">
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
       <c r="S22" s="14">

</xml_diff>